<commit_message>
bi: updae the electronic forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Burundi/bi_oncho_prestop_3_202307_diag.xlsx
+++ b/ONCHO/Impact Assessments/Burundi/bi_oncho_prestop_3_202307_diag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Burundi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0FB522-E56F-4747-832F-F5C9364F8325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4320448F-4308-4EBF-96DF-91F568C6A3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="120">
   <si>
     <t>form_title</t>
   </si>
@@ -209,9 +209,6 @@
     <t>yes_no</t>
   </si>
   <si>
-    <t>select_one yes_no</t>
-  </si>
-  <si>
     <t>Positif</t>
   </si>
   <si>
@@ -257,27 +254,6 @@
     <t>Entrer le nom du village</t>
   </si>
   <si>
-    <t>d_ov16_result_1</t>
-  </si>
-  <si>
-    <t>d_ov16_result_2</t>
-  </si>
-  <si>
-    <t>Résultat OV16 du test 2</t>
-  </si>
-  <si>
-    <t>d_control_1</t>
-  </si>
-  <si>
-    <t>Ligne de contrôle positive visible du test 1</t>
-  </si>
-  <si>
-    <t>Résultat OV16 du test 1</t>
-  </si>
-  <si>
-    <t>Ligne de contrôle positive visible du test 2</t>
-  </si>
-  <si>
     <t>d_elisa_result</t>
   </si>
   <si>
@@ -305,9 +281,6 @@
     <t>Le code répéter doit être le même</t>
   </si>
   <si>
-    <t>d_control_2</t>
-  </si>
-  <si>
     <t>select_one region_list</t>
   </si>
   <si>
@@ -332,45 +305,12 @@
     <t>ELISA - Décision final (test2)</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>d_est_invalide_1</t>
-  </si>
-  <si>
-    <t>Le résultat est invalide parce que la contrôle est non visible</t>
-  </si>
-  <si>
-    <t>${d_control_1} = 'Non'</t>
-  </si>
-  <si>
-    <t>${d_control_1} = 'Oui'</t>
-  </si>
-  <si>
-    <t>d_est_invalide_2</t>
-  </si>
-  <si>
-    <t>${d_control_2} = 'Non'</t>
-  </si>
-  <si>
-    <t>${d_ov16_result_1} = 'Indéterminé' or ${d_control_1} = 'Non'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ${d_control_2} = 'Oui'</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ${d_elisa_result} = 'Indéterminé'</t>
   </si>
   <si>
-    <t>(${d_ov16_result_1} != 'Indéterminé' or  ${d_ov16_result_2} != 'Indéterminé' ) and ( ${d_control_1} = 'Oui' or ${d_control_2} = 'Oui')</t>
-  </si>
-  <si>
     <t>bi_oncho_prestop_3_202307_diag</t>
   </si>
   <si>
-    <t>(2023 Juillet) ONCHO pre Stop - 3. Résultats de laboratoire V2.2</t>
-  </si>
-  <si>
     <t>BUBANZA</t>
   </si>
   <si>
@@ -447,6 +387,9 @@
   </si>
   <si>
     <t>MUHEKA</t>
+  </si>
+  <si>
+    <t>(2023 Juillet) ONCHO pre Stop - 3. Résultats de laboratoire</t>
   </si>
 </sst>
 </file>
@@ -916,13 +859,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1009,10 +952,10 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>34</v>
@@ -1037,7 +980,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="15"/>
@@ -1050,7 +993,7 @@
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="14" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1061,7 +1004,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="15"/>
@@ -1079,13 +1022,13 @@
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="15"/>
@@ -1104,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>57</v>
@@ -1114,7 +1057,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="12"/>
       <c r="H7" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="9" t="s">
@@ -1128,21 +1071,21 @@
         <v>24</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="15"/>
       <c r="F8" s="22" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="9" t="s">
@@ -1166,7 +1109,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="16"/>
       <c r="H9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="21" t="s">
@@ -1175,306 +1118,160 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" s="13"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="13"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="13" t="s">
-        <v>104</v>
+      <c r="H12" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="J12" s="21"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="19" t="s">
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="I13" s="9"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-    </row>
-    <row r="18" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-    </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-    </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B15" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B16" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-    </row>
-    <row r="23" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1486,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD48"/>
     </sheetView>
@@ -1575,46 +1372,46 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="C10" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1622,13 +1419,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1680,10 +1477,10 @@
         <v>33</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1694,10 +1491,10 @@
         <v>33</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1708,10 +1505,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1722,10 +1519,10 @@
         <v>33</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1736,10 +1533,10 @@
         <v>33</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1750,10 +1547,10 @@
         <v>33</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1772,13 +1569,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1788,13 +1585,13 @@
         <v>18</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1804,13 +1601,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1820,13 +1617,13 @@
         <v>18</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1836,13 +1633,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1852,13 +1649,13 @@
         <v>18</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1868,13 +1665,13 @@
         <v>18</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1884,13 +1681,13 @@
         <v>18</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1900,13 +1697,13 @@
         <v>18</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1916,13 +1713,13 @@
         <v>18</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1940,14 +1737,14 @@
         <v>35</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -1956,14 +1753,14 @@
         <v>35</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -1972,14 +1769,14 @@
         <v>35</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -1988,14 +1785,14 @@
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -2004,14 +1801,14 @@
         <v>35</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -2020,14 +1817,14 @@
         <v>35</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -2036,14 +1833,14 @@
         <v>35</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -2052,14 +1849,14 @@
         <v>35</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -2068,14 +1865,14 @@
         <v>35</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -2084,14 +1881,14 @@
         <v>35</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F43" s="3"/>
     </row>
@@ -2100,14 +1897,14 @@
         <v>35</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -2116,14 +1913,14 @@
         <v>35</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F45" s="3"/>
     </row>
@@ -2132,14 +1929,14 @@
         <v>35</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F46" s="3"/>
     </row>
@@ -2148,14 +1945,14 @@
         <v>35</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F47" s="3"/>
     </row>
@@ -2164,14 +1961,14 @@
         <v>35</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -2323,7 +2120,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2348,10 +2145,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>

</xml_diff>